<commit_message>
retweak of separation parameters with cubic spline fit
</commit_message>
<xml_diff>
--- a/docs/Examples/Example1a_Gas_Cell_Calibration/Discarded_df.xlsx
+++ b/docs/Examples/Example1a_Gas_Cell_Calibration/Discarded_df.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>filename</t>
   </si>
@@ -95,6 +95,12 @@
   </si>
   <si>
     <t>Mean_HB_prom</t>
+  </si>
+  <si>
+    <t>Diad2_prom/std_betweendiads</t>
+  </si>
+  <si>
+    <t>Left_vs_Right</t>
   </si>
 </sst>
 </file>
@@ -452,13 +458,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:AB1"/>
+  <dimension ref="B1:AD1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="2:28">
+    <row r="1" spans="2:30">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -539,6 +545,12 @@
       </c>
       <c r="AB1" s="1" t="s">
         <v>26</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Renamed CO2_density_gcm3 to CO2_dens_gcm3, changed density_gcm3 to specify CO2, tweaked parameter looping
</commit_message>
<xml_diff>
--- a/docs/Examples/Example1a_Gas_Cell_Calibration/Discarded_df.xlsx
+++ b/docs/Examples/Example1a_Gas_Cell_Calibration/Discarded_df.xlsx
@@ -14,93 +14,105 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
   <si>
     <t>filename</t>
   </si>
   <si>
-    <t>Diad2_HB2_prom_ratio</t>
-  </si>
-  <si>
-    <t>Diad1_HB1_prom_ratio</t>
+    <t>approx_split</t>
+  </si>
+  <si>
+    <t>Diad1_pos</t>
   </si>
   <si>
     <t>Diad2_pos</t>
   </si>
   <si>
-    <t>Diad2_prom</t>
-  </si>
-  <si>
-    <t>Diad1_pos</t>
-  </si>
-  <si>
-    <t>Diad1_prom</t>
+    <t>HB1_pos</t>
   </si>
   <si>
     <t>HB2_pos</t>
   </si>
   <si>
-    <t>HB2_prom</t>
-  </si>
-  <si>
-    <t>HB1_pos</t>
-  </si>
-  <si>
-    <t>HB1_prom</t>
-  </si>
-  <si>
     <t>C13_pos</t>
   </si>
   <si>
-    <t>C13_prom</t>
+    <t>Diad1_abs_prom</t>
+  </si>
+  <si>
+    <t>Diad2_abs_prom</t>
+  </si>
+  <si>
+    <t>HB1_abs_prom</t>
+  </si>
+  <si>
+    <t>HB2_abs_prom</t>
+  </si>
+  <si>
+    <t>C13_abs_prom</t>
+  </si>
+  <si>
+    <t>Mean_abs_HB_prom</t>
+  </si>
+  <si>
+    <t>Diad2_HB2_abs_prom_ratio</t>
+  </si>
+  <si>
+    <t>Diad1_HB1_abs_prom_ratio</t>
+  </si>
+  <si>
+    <t>Diad1_rel_prom</t>
+  </si>
+  <si>
+    <t>Diad2_rel_prom</t>
+  </si>
+  <si>
+    <t>HB1_rel_prom</t>
+  </si>
+  <si>
+    <t>HB2_rel_prom</t>
+  </si>
+  <si>
+    <t>C13_rel_prom</t>
+  </si>
+  <si>
+    <t>Diad1_HB1_Valley_prom</t>
+  </si>
+  <si>
+    <t>Mean_Diad_HB_Valley_prom</t>
   </si>
   <si>
     <t>Diad1_prom/std_betweendiads</t>
   </si>
   <si>
+    <t>Diad2_prom/std_betweendiads</t>
+  </si>
+  <si>
     <t>Diad2_height</t>
   </si>
   <si>
     <t>HB2_height</t>
   </si>
   <si>
+    <t>C13_height</t>
+  </si>
+  <si>
+    <t>Diad1_height</t>
+  </si>
+  <si>
+    <t>HB1_height</t>
+  </si>
+  <si>
+    <t>Diad1_Median_Bck</t>
+  </si>
+  <si>
+    <t>Diad2_Median_Bck</t>
+  </si>
+  <si>
+    <t>C13_HB2_abs_prom_ratio</t>
+  </si>
+  <si>
     <t>Diad2_HB2_Valley_prom</t>
-  </si>
-  <si>
-    <t>C13_height</t>
-  </si>
-  <si>
-    <t>Diad1_height</t>
-  </si>
-  <si>
-    <t>HB1_height</t>
-  </si>
-  <si>
-    <t>Diad1_HB1_Valley_prom</t>
-  </si>
-  <si>
-    <t>Diad1_Median_Bck</t>
-  </si>
-  <si>
-    <t>Diad2_Median_Bck</t>
-  </si>
-  <si>
-    <t>approx_split</t>
-  </si>
-  <si>
-    <t>C13_HB2_prom_ratio</t>
-  </si>
-  <si>
-    <t>Mean_Diad_HB_Valley_prom</t>
-  </si>
-  <si>
-    <t>Mean_HB_prom</t>
-  </si>
-  <si>
-    <t>Diad2_prom/std_betweendiads</t>
-  </si>
-  <si>
-    <t>Left_vs_Right</t>
   </si>
 </sst>
 </file>
@@ -458,13 +470,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:AD1"/>
+  <dimension ref="B1:AL1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="2:30">
+    <row r="1" spans="2:38">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -526,31 +538,55 @@
         <v>19</v>
       </c>
       <c r="V1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>28</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixing secondary phases to work with CRR Code
</commit_message>
<xml_diff>
--- a/docs/Examples/Example1a_Gas_Cell_Calibration/Discarded_df.xlsx
+++ b/docs/Examples/Example1a_Gas_Cell_Calibration/Discarded_df.xlsx
@@ -14,11 +14,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
   <si>
     <t>filename</t>
   </si>
   <si>
+    <t>rays_present</t>
+  </si>
+  <si>
     <t>approx_split</t>
   </si>
   <si>
@@ -86,6 +89,15 @@
   </si>
   <si>
     <t>Diad2_prom/std_betweendiads</t>
+  </si>
+  <si>
+    <t>Av_Diad_prom/std_betweendiads</t>
+  </si>
+  <si>
+    <t>C13_prom/HB2_prom</t>
+  </si>
+  <si>
+    <t>Av_Diad_HB_prom_ratio</t>
   </si>
   <si>
     <t>Diad2_height</t>
@@ -470,13 +482,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:AL1"/>
+  <dimension ref="B1:AP1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="2:38">
+    <row r="1" spans="2:42">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -538,25 +550,25 @@
         <v>19</v>
       </c>
       <c r="V1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="AC1" s="1" t="s">
         <v>23</v>
@@ -587,6 +599,18 @@
       </c>
       <c r="AL1" s="1" t="s">
         <v>32</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pushed Berenise and Raela's comments
</commit_message>
<xml_diff>
--- a/docs/Examples/Example1a_Gas_Cell_Calibration/Discarded_df.xlsx
+++ b/docs/Examples/Example1a_Gas_Cell_Calibration/Discarded_df.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>filename</t>
   </si>
@@ -100,6 +100,9 @@
     <t>Av_Diad_HB_prom_ratio</t>
   </si>
   <si>
+    <t>Left_vs_Right</t>
+  </si>
+  <si>
     <t>Diad2_height</t>
   </si>
   <si>
@@ -125,6 +128,12 @@
   </si>
   <si>
     <t>Diad2_HB2_Valley_prom</t>
+  </si>
+  <si>
+    <t>HB1_prom/std_betweendiads</t>
+  </si>
+  <si>
+    <t>HB2_prom/std_betweendiads</t>
   </si>
 </sst>
 </file>
@@ -482,13 +491,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:AP1"/>
+  <dimension ref="B1:AO1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="2:42">
+    <row r="1" spans="2:41">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -553,64 +562,61 @@
         <v>20</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>